<commit_message>
added empatica file splitter for test with adri and leile
</commit_message>
<xml_diff>
--- a/score_and_help_indicator.xlsx
+++ b/score_and_help_indicator.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="172">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -509,6 +509,33 @@
   </si>
   <si>
     <t xml:space="preserve">9:41:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adriana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A02F50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adriana4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adriana2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adriana1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leichtle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leichtle4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leichtle2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leichtle1</t>
   </si>
 </sst>
 </file>
@@ -620,14 +647,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC13"/>
+  <dimension ref="A1:AC23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.28"/>
   </cols>
   <sheetData>
@@ -1788,6 +1816,71 @@
         <v>8</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.700694444444444" right="0.700694444444444" top="0.752083333333333" bottom="0.752083333333333" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>